<commit_message>
Revue 2, first test module
</commit_message>
<xml_diff>
--- a/Revue 1/BonCommande_Parking.xlsx
+++ b/Revue 1/BonCommande_Parking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>BON DE COMMANDE 2023-2024 N° 01</t>
   </si>
@@ -58,7 +58,7 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t>Date d'envoi :   18</t>
+      <t>Date d'envoi :   22</t>
     </r>
     <r>
       <rPr>
@@ -67,7 +67,7 @@
         <color theme="1"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve"> / 02 /2024</t>
+      <t xml:space="preserve"> / 03 /2024</t>
     </r>
   </si>
   <si>
@@ -104,44 +104,19 @@
     <t>MC</t>
   </si>
   <si>
-    <t>https://fr.rs-online.com/web/p/capteurs-photoelectriques/7525180?redirect-relevancy-data=7365617263685F636173636164655F6F726465723D31267365617263685F696E746572666163655F6E616D653D4931384E53656172636847656E65726963267365617263685F6D617463685F6D6F64653D6D61746368616C6C7061727469616C267365617263685F7061747465726E5F6D6174636865643D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B24267365617263685F747970653D4B4559574F52445F53494E474C455F414C5048415F4E554D45524943267365617263685F7370656C6C5F636F72726563745F6170706C6965643D59267365617263685F77696C645F63617264696E675F6D6F64653D4E4F4E45267365617263685F6B6579776F72643D585542324250414E4C3252267365617263685F6B6579776F72645F6170703D585542324250414E4C325226</t>
+    <t>https://www.europ-camera.fr/1962-camera-ip-hikvision-dome-ds-2cd1143g2-i-4mp-h265-objectif-28mm-vision-nocturne-30m-poe-onvif.html</t>
   </si>
   <si>
-    <t xml:space="preserve">XUB2BPANL2R
-</t>
+    <t>DS-2CD1143G2-I</t>
   </si>
   <si>
-    <t>RS</t>
+    <t>HIKVISION</t>
   </si>
   <si>
     <t>SI-NSI</t>
   </si>
   <si>
-    <t>https://www.lextronic.fr/convertisseur-tcp-ip-rs232-8-entrees-8-sorties-cie-h10a-59843.html</t>
-  </si>
-  <si>
-    <t>CIE-H10A</t>
-  </si>
-  <si>
-    <t>Lextronic</t>
-  </si>
-  <si>
-    <t>https://www.hikdistribution.com/fr/products/hikvision-ds-2cd2085g1-i-4k-alimentaire-par-darkfighter-mini-camera-reseau-de-puces</t>
-  </si>
-  <si>
-    <t>DS-2CD2085G1-I</t>
-  </si>
-  <si>
-    <t>Hikdistribution</t>
-  </si>
-  <si>
     <t>BTS ELEC</t>
-  </si>
-  <si>
-    <t>https://www.alternate.fr/Philips-Hue/A60-Ampoule-connect%C3%A9e-E27-800-(lot-de-2)-Lampe-%C3%A0-LED/html/product/1791961?partner=FrIdealo&amp;campaign=Lampe/Philips+Hue/1791961</t>
-  </si>
-  <si>
-    <t>Alternate</t>
   </si>
   <si>
     <t>UFA BTS MS</t>
@@ -222,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -323,7 +298,7 @@
     <font>
       <u/>
       <sz val="11.0"/>
-      <color rgb="FF56A3F1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -336,12 +311,6 @@
       <u/>
       <sz val="11.0"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11.0"/>
-      <color rgb="FF56A3F1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -752,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -833,7 +802,7 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
@@ -842,12 +811,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="22" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="19" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -864,27 +848,6 @@
     </xf>
     <xf borderId="21" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="22" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="19" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="21" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -926,7 +889,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="35" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1584,7 +1547,7 @@
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="39">
-        <v>81.8</v>
+        <v>98.28</v>
       </c>
       <c r="I12" s="40">
         <v>1.0</v>
@@ -1593,8 +1556,8 @@
         <v>1.0</v>
       </c>
       <c r="K12" s="41">
-        <f t="shared" ref="K12:K17" si="1">H12*J12</f>
-        <v>81.8</v>
+        <f>H12*J12</f>
+        <v>98.28</v>
       </c>
       <c r="L12" s="42" t="s">
         <v>25</v>
@@ -1618,34 +1581,19 @@
       <c r="A13" s="23">
         <v>2.0</v>
       </c>
-      <c r="B13" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="B13" s="44"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="45" t="s">
-        <v>28</v>
-      </c>
+      <c r="F13" s="45"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="46">
-        <v>202.8</v>
-      </c>
-      <c r="I13" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="J13" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="K13" s="48">
-        <f t="shared" si="1"/>
-        <v>202.8</v>
-      </c>
-      <c r="L13" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="23"/>
-      <c r="N13" s="50"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="46"/>
       <c r="O13" s="23"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -1663,40 +1611,25 @@
       <c r="A14" s="23">
         <v>3.0</v>
       </c>
-      <c r="B14" s="51" t="s">
-        <v>30</v>
-      </c>
+      <c r="B14" s="44"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="52" t="s">
-        <v>31</v>
-      </c>
+      <c r="F14" s="45"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="39">
-        <v>141.95</v>
-      </c>
-      <c r="I14" s="40">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="40">
-        <v>1.0</v>
-      </c>
-      <c r="K14" s="41">
-        <f t="shared" si="1"/>
-        <v>141.95</v>
-      </c>
-      <c r="L14" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="23"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="18"/>
       <c r="N14" s="43"/>
       <c r="O14" s="23"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="S14" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
@@ -1708,40 +1641,25 @@
       <c r="A15" s="23">
         <v>4.0</v>
       </c>
-      <c r="B15" s="53" t="s">
-        <v>34</v>
-      </c>
+      <c r="B15" s="44"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="54">
-        <v>1791961.0</v>
-      </c>
+      <c r="F15" s="45"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="55">
-        <v>47.79</v>
-      </c>
-      <c r="I15" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="J15" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="K15" s="48">
-        <f t="shared" si="1"/>
-        <v>47.79</v>
-      </c>
-      <c r="L15" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" s="23"/>
-      <c r="N15" s="50"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="46"/>
       <c r="O15" s="23"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="S15" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="T15" s="14"/>
       <c r="U15" s="14"/>
@@ -1753,20 +1671,20 @@
       <c r="A16" s="23">
         <v>5.0</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="52"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="39"/>
+      <c r="H16" s="47"/>
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K16:K17" si="1">H16*J16</f>
         <v>0</v>
       </c>
-      <c r="L16" s="42"/>
+      <c r="L16" s="48"/>
       <c r="M16" s="23"/>
       <c r="N16" s="43"/>
       <c r="O16" s="23"/>
@@ -1774,7 +1692,7 @@
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
       <c r="S16" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="T16" s="14"/>
       <c r="U16" s="14"/>
@@ -1786,28 +1704,28 @@
       <c r="A17" s="23">
         <v>6.0</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="45"/>
+      <c r="F17" s="50"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48">
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="54"/>
       <c r="M17" s="23"/>
-      <c r="N17" s="50"/>
+      <c r="N17" s="46"/>
       <c r="O17" s="23"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="S17" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
@@ -1819,19 +1737,19 @@
       <c r="A18" s="23">
         <v>7.0</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="52"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="39"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
       <c r="K18" s="41">
         <v>0.0</v>
       </c>
-      <c r="L18" s="42"/>
+      <c r="L18" s="48"/>
       <c r="M18" s="23"/>
       <c r="N18" s="43"/>
       <c r="O18" s="23"/>
@@ -1839,7 +1757,7 @@
       <c r="Q18" s="14"/>
       <c r="R18" s="14"/>
       <c r="S18" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="T18" s="14"/>
       <c r="U18" s="14"/>
@@ -1851,27 +1769,27 @@
       <c r="A19" s="23">
         <v>8.0</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="45"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="48">
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53">
         <v>0.0</v>
       </c>
-      <c r="L19" s="49"/>
+      <c r="L19" s="54"/>
       <c r="M19" s="23"/>
-      <c r="N19" s="50"/>
+      <c r="N19" s="46"/>
       <c r="O19" s="23"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
       <c r="S19" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="T19" s="14"/>
       <c r="U19" s="14"/>
@@ -1883,20 +1801,20 @@
       <c r="A20" s="23">
         <v>9.0</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="52"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="39"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="41">
         <f t="shared" ref="K20:K33" si="2">H20*J20</f>
         <v>0</v>
       </c>
-      <c r="L20" s="42"/>
+      <c r="L20" s="48"/>
       <c r="M20" s="23"/>
       <c r="N20" s="43"/>
       <c r="O20" s="23"/>
@@ -1904,7 +1822,7 @@
       <c r="Q20" s="14"/>
       <c r="R20" s="14"/>
       <c r="S20" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="T20" s="14"/>
       <c r="U20" s="14"/>
@@ -1916,22 +1834,22 @@
       <c r="A21" s="23">
         <v>10.0</v>
       </c>
-      <c r="B21" s="58"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="45"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="48">
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L21" s="49"/>
+      <c r="L21" s="54"/>
       <c r="M21" s="23"/>
-      <c r="N21" s="50"/>
+      <c r="N21" s="46"/>
       <c r="O21" s="23"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -1947,20 +1865,20 @@
       <c r="A22" s="23">
         <v>11.0</v>
       </c>
-      <c r="B22" s="57"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="52"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="18"/>
-      <c r="H22" s="39"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
       <c r="K22" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L22" s="42"/>
+      <c r="L22" s="48"/>
       <c r="M22" s="23"/>
       <c r="N22" s="43"/>
       <c r="O22" s="23"/>
@@ -1978,22 +1896,22 @@
       <c r="A23" s="23">
         <v>12.0</v>
       </c>
-      <c r="B23" s="58"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="45"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="18"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="48">
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L23" s="49"/>
+      <c r="L23" s="54"/>
       <c r="M23" s="23"/>
-      <c r="N23" s="50"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="23"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -2009,20 +1927,20 @@
       <c r="A24" s="23">
         <v>13.0</v>
       </c>
-      <c r="B24" s="57"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="52"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="39"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="K24" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L24" s="42"/>
+      <c r="L24" s="48"/>
       <c r="M24" s="23"/>
       <c r="N24" s="43"/>
       <c r="O24" s="23"/>
@@ -2040,28 +1958,28 @@
       <c r="A25" s="23">
         <v>14.0</v>
       </c>
-      <c r="B25" s="58"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="45"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="48">
+      <c r="H25" s="51"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L25" s="49"/>
+      <c r="L25" s="54"/>
       <c r="M25" s="23"/>
-      <c r="N25" s="50"/>
+      <c r="N25" s="46"/>
       <c r="O25" s="23"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="T25" s="14"/>
       <c r="U25" s="14"/>
@@ -2073,20 +1991,20 @@
       <c r="A26" s="23">
         <v>15.0</v>
       </c>
-      <c r="B26" s="57"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="52"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="39"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="40"/>
       <c r="J26" s="40"/>
       <c r="K26" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L26" s="42"/>
+      <c r="L26" s="48"/>
       <c r="M26" s="23"/>
       <c r="N26" s="43"/>
       <c r="O26" s="23"/>
@@ -2094,7 +2012,7 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="T26" s="14"/>
       <c r="U26" s="14"/>
@@ -2106,28 +2024,28 @@
       <c r="A27" s="23">
         <v>16.0</v>
       </c>
-      <c r="B27" s="58"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="45"/>
+      <c r="F27" s="50"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="48">
+      <c r="H27" s="51"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="49"/>
+      <c r="L27" s="54"/>
       <c r="M27" s="23"/>
-      <c r="N27" s="50"/>
+      <c r="N27" s="46"/>
       <c r="O27" s="23"/>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
       <c r="R27" s="14"/>
       <c r="S27" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="T27" s="14"/>
       <c r="U27" s="14"/>
@@ -2139,20 +2057,20 @@
       <c r="A28" s="23">
         <v>17.0</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="52"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="39"/>
+      <c r="H28" s="47"/>
       <c r="I28" s="40"/>
       <c r="J28" s="40"/>
       <c r="K28" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L28" s="42"/>
+      <c r="L28" s="48"/>
       <c r="M28" s="23"/>
       <c r="N28" s="43"/>
       <c r="O28" s="23"/>
@@ -2160,7 +2078,7 @@
       <c r="Q28" s="14"/>
       <c r="R28" s="14"/>
       <c r="S28" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="T28" s="14"/>
       <c r="U28" s="14"/>
@@ -2172,28 +2090,28 @@
       <c r="A29" s="23">
         <v>18.0</v>
       </c>
-      <c r="B29" s="58"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="18"/>
-      <c r="F29" s="45"/>
+      <c r="F29" s="50"/>
       <c r="G29" s="18"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48">
+      <c r="H29" s="51"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L29" s="49"/>
+      <c r="L29" s="54"/>
       <c r="M29" s="23"/>
-      <c r="N29" s="50"/>
+      <c r="N29" s="46"/>
       <c r="O29" s="23"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
       <c r="S29" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="T29" s="14"/>
       <c r="U29" s="14"/>
@@ -2205,20 +2123,20 @@
       <c r="A30" s="23">
         <v>19.0</v>
       </c>
-      <c r="B30" s="57"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
-      <c r="F30" s="52"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="18"/>
-      <c r="H30" s="39"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="40"/>
       <c r="J30" s="40"/>
       <c r="K30" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L30" s="42"/>
+      <c r="L30" s="48"/>
       <c r="M30" s="23"/>
       <c r="N30" s="43"/>
       <c r="O30" s="23"/>
@@ -2236,22 +2154,22 @@
       <c r="A31" s="23">
         <v>20.0</v>
       </c>
-      <c r="B31" s="58"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="45"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="18"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="48">
+      <c r="H31" s="51"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L31" s="49"/>
+      <c r="L31" s="54"/>
       <c r="M31" s="23"/>
-      <c r="N31" s="50"/>
+      <c r="N31" s="46"/>
       <c r="O31" s="23"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
@@ -2267,20 +2185,20 @@
       <c r="A32" s="23">
         <v>21.0</v>
       </c>
-      <c r="B32" s="57"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="18"/>
-      <c r="F32" s="52"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="18"/>
-      <c r="H32" s="39"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="40"/>
       <c r="J32" s="40"/>
       <c r="K32" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L32" s="42"/>
+      <c r="L32" s="48"/>
       <c r="M32" s="23"/>
       <c r="N32" s="43"/>
       <c r="O32" s="23"/>
@@ -2298,22 +2216,22 @@
       <c r="A33" s="23">
         <v>22.0</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="65">
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="63">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L33" s="66"/>
+      <c r="L33" s="64"/>
       <c r="M33" s="23"/>
-      <c r="N33" s="67"/>
+      <c r="N33" s="65"/>
       <c r="O33" s="23"/>
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
@@ -2326,18 +2244,18 @@
       <c r="X33" s="23"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="68"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="71" t="s">
-        <v>47</v>
+      <c r="B34" s="66"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="69" t="s">
+        <v>39</v>
       </c>
       <c r="I34" s="26"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="73">
+      <c r="J34" s="70"/>
+      <c r="K34" s="71">
         <f>SUM(K12:K33)</f>
-        <v>474.34</v>
+        <v>98.28</v>
       </c>
       <c r="M34" s="23"/>
       <c r="N34" s="23"/>
@@ -2350,11 +2268,11 @@
       <c r="U34" s="14"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="75" t="s">
-        <v>49</v>
+      <c r="B35" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>41</v>
       </c>
       <c r="M35" s="23"/>
       <c r="N35" s="23"/>
@@ -2378,7 +2296,7 @@
       <c r="I36" s="23"/>
       <c r="J36" s="23"/>
       <c r="K36" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="M36" s="23"/>
       <c r="N36" s="23"/>
@@ -2417,7 +2335,7 @@
       <c r="A38" s="23"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="23"/>
@@ -2490,14 +2408,14 @@
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
       <c r="E41" s="23" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
       <c r="J41" s="23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
@@ -5388,42 +5306,26 @@
       <c r="S1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="F2:K3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:I9"/>
+  <mergeCells count="66">
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="B26:E26"/>
@@ -5446,18 +5348,40 @@
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F2:K3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="L5"/>
     <hyperlink r:id="rId2" ref="B12"/>
-    <hyperlink r:id="rId3" ref="B13"/>
-    <hyperlink r:id="rId4" ref="B14"/>
-    <hyperlink r:id="rId5" ref="B15"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="landscape"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>